<commit_message>
feat: fill required columns
</commit_message>
<xml_diff>
--- a/examples/download.xlsx
+++ b/examples/download.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="199">
   <si>
     <t>訂單號碼
 Số phiếu giao</t>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>ăn sáng</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
   <si>
     <t>C.NGOAN</t>
@@ -1069,19 +1072,19 @@
         <v>67</v>
       </c>
       <c r="H2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -1104,19 +1107,19 @@
         <v>68</v>
       </c>
       <c r="H3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1139,19 +1142,22 @@
         <v>69</v>
       </c>
       <c r="H4" t="s">
-        <v>93</v>
+        <v>94</v>
+      </c>
+      <c r="I4" t="s">
+        <v>86</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="O4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1174,19 +1180,22 @@
         <v>70</v>
       </c>
       <c r="H5" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+      <c r="I5" t="s">
+        <v>86</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="O5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1209,19 +1218,22 @@
         <v>70</v>
       </c>
       <c r="H6" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+      <c r="I6" t="s">
+        <v>86</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="O6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1244,19 +1256,22 @@
         <v>71</v>
       </c>
       <c r="H7" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+      <c r="I7" t="s">
+        <v>86</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="O7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1279,19 +1294,22 @@
         <v>72</v>
       </c>
       <c r="H8" t="s">
-        <v>95</v>
+        <v>96</v>
+      </c>
+      <c r="I8" t="s">
+        <v>86</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1314,16 +1332,19 @@
         <v>73</v>
       </c>
       <c r="H9" t="s">
-        <v>96</v>
+        <v>97</v>
+      </c>
+      <c r="I9" t="s">
+        <v>86</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1346,19 +1367,22 @@
         <v>74</v>
       </c>
       <c r="H10" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="I10" t="s">
+        <v>86</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="O10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1381,19 +1405,22 @@
         <v>74</v>
       </c>
       <c r="H11" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="I11" t="s">
+        <v>86</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="O11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1416,19 +1443,22 @@
         <v>74</v>
       </c>
       <c r="H12" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="I12" t="s">
+        <v>86</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="O12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1451,19 +1481,22 @@
         <v>74</v>
       </c>
       <c r="H13" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="I13" t="s">
+        <v>86</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="O13" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1486,19 +1519,22 @@
         <v>74</v>
       </c>
       <c r="H14" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="I14" t="s">
+        <v>86</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="O14" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1521,19 +1557,22 @@
         <v>74</v>
       </c>
       <c r="H15" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="I15" t="s">
+        <v>86</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="O15" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1556,19 +1595,22 @@
         <v>74</v>
       </c>
       <c r="H16" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="I16" t="s">
+        <v>86</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N16" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="O16" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1591,16 +1633,19 @@
         <v>75</v>
       </c>
       <c r="H17" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="I17" t="s">
+        <v>86</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1623,19 +1668,19 @@
         <v>76</v>
       </c>
       <c r="H18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I18" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1658,19 +1703,22 @@
         <v>77</v>
       </c>
       <c r="H19" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="I19" t="s">
+        <v>86</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="O19" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1693,19 +1741,22 @@
         <v>77</v>
       </c>
       <c r="H20" t="s">
-        <v>101</v>
+        <v>102</v>
+      </c>
+      <c r="I20" t="s">
+        <v>86</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N20" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O20" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -1728,19 +1779,22 @@
         <v>78</v>
       </c>
       <c r="H21" t="s">
-        <v>93</v>
+        <v>94</v>
+      </c>
+      <c r="I21" t="s">
+        <v>86</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N21" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="O21" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1763,19 +1817,22 @@
         <v>77</v>
       </c>
       <c r="H22" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="I22" t="s">
+        <v>86</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N22" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="O22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1798,19 +1855,22 @@
         <v>78</v>
       </c>
       <c r="H23" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="I23" t="s">
+        <v>86</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="O23" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1833,19 +1893,22 @@
         <v>72</v>
       </c>
       <c r="H24" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="I24" t="s">
+        <v>86</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N24" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="O24" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -1868,19 +1931,22 @@
         <v>79</v>
       </c>
       <c r="H25" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="I25" t="s">
+        <v>86</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="O25" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -1903,19 +1969,22 @@
         <v>70</v>
       </c>
       <c r="H26" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+      <c r="I26" t="s">
+        <v>86</v>
       </c>
       <c r="L26">
         <v>0</v>
       </c>
       <c r="M26" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N26" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="O26" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -1938,19 +2007,22 @@
         <v>80</v>
       </c>
       <c r="H27" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="I27" t="s">
+        <v>86</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N27" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="O27" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -1973,16 +2045,19 @@
         <v>81</v>
       </c>
       <c r="H28" t="s">
-        <v>103</v>
+        <v>104</v>
+      </c>
+      <c r="I28" t="s">
+        <v>86</v>
       </c>
       <c r="L28">
         <v>0</v>
       </c>
       <c r="M28" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N28" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -2005,19 +2080,22 @@
         <v>77</v>
       </c>
       <c r="H29" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="I29" t="s">
+        <v>86</v>
       </c>
       <c r="L29">
         <v>0</v>
       </c>
       <c r="M29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N29" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="O29" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -2040,19 +2118,22 @@
         <v>77</v>
       </c>
       <c r="H30" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="I30" t="s">
+        <v>86</v>
       </c>
       <c r="L30">
         <v>0</v>
       </c>
       <c r="M30" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N30" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O30" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -2075,19 +2156,22 @@
         <v>77</v>
       </c>
       <c r="H31" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="I31" t="s">
+        <v>86</v>
       </c>
       <c r="L31">
         <v>0</v>
       </c>
       <c r="M31" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N31" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="O31" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -2110,19 +2194,22 @@
         <v>82</v>
       </c>
       <c r="H32" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="I32" t="s">
+        <v>86</v>
       </c>
       <c r="L32">
         <v>0</v>
       </c>
       <c r="M32" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N32" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="O32" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -2145,19 +2232,22 @@
         <v>82</v>
       </c>
       <c r="H33" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="I33" t="s">
+        <v>86</v>
       </c>
       <c r="L33">
         <v>0</v>
       </c>
       <c r="M33" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N33" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="O33" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -2180,19 +2270,22 @@
         <v>82</v>
       </c>
       <c r="H34" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="I34" t="s">
+        <v>86</v>
       </c>
       <c r="L34">
         <v>0</v>
       </c>
       <c r="M34" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N34" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="O34" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:15">
@@ -2215,22 +2308,22 @@
         <v>83</v>
       </c>
       <c r="H35" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I35" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="L35">
         <v>0</v>
       </c>
       <c r="M35" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N35" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="O35" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="36" spans="1:15">
@@ -2253,19 +2346,19 @@
         <v>84</v>
       </c>
       <c r="H36" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I36" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L36">
         <v>0</v>
       </c>
       <c r="M36" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N36" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:15">
@@ -2288,16 +2381,19 @@
         <v>85</v>
       </c>
       <c r="H37" t="s">
-        <v>107</v>
+        <v>108</v>
+      </c>
+      <c r="I37" t="s">
+        <v>86</v>
       </c>
       <c r="L37">
         <v>0</v>
       </c>
       <c r="M37" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N37" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:15">
@@ -2320,16 +2416,19 @@
         <v>73</v>
       </c>
       <c r="H38" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="I38" t="s">
+        <v>86</v>
       </c>
       <c r="L38">
         <v>0</v>
       </c>
       <c r="M38" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N38" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:15">
@@ -2348,14 +2447,20 @@
       <c r="F39" t="s">
         <v>61</v>
       </c>
+      <c r="G39" t="s">
+        <v>86</v>
+      </c>
+      <c r="I39" t="s">
+        <v>86</v>
+      </c>
       <c r="L39">
         <v>1707160</v>
       </c>
       <c r="M39" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N39" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:15">
@@ -2375,19 +2480,22 @@
         <v>63</v>
       </c>
       <c r="G40" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H40" t="s">
-        <v>109</v>
+        <v>110</v>
+      </c>
+      <c r="I40" t="s">
+        <v>86</v>
       </c>
       <c r="L40">
         <v>0</v>
       </c>
       <c r="M40" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:15">
@@ -2407,19 +2515,22 @@
         <v>63</v>
       </c>
       <c r="G41" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H41" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="I41" t="s">
+        <v>86</v>
       </c>
       <c r="L41">
         <v>0</v>
       </c>
       <c r="M41" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:15">
@@ -2442,16 +2553,19 @@
         <v>78</v>
       </c>
       <c r="H42" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="I42" t="s">
+        <v>86</v>
       </c>
       <c r="L42">
         <v>0</v>
       </c>
       <c r="M42" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N42" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:15">
@@ -2474,16 +2588,19 @@
         <v>70</v>
       </c>
       <c r="H43" t="s">
-        <v>112</v>
+        <v>113</v>
+      </c>
+      <c r="I43" t="s">
+        <v>86</v>
       </c>
       <c r="L43">
         <v>0</v>
       </c>
       <c r="M43" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:15">
@@ -2503,19 +2620,22 @@
         <v>61</v>
       </c>
       <c r="G44" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H44" t="s">
-        <v>113</v>
+        <v>114</v>
+      </c>
+      <c r="I44" t="s">
+        <v>86</v>
       </c>
       <c r="L44">
         <v>0</v>
       </c>
       <c r="M44" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N44" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:15">
@@ -2535,22 +2655,22 @@
         <v>61</v>
       </c>
       <c r="G45" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H45" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I45" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L45">
         <v>0</v>
       </c>
       <c r="M45" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N45" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:15">
@@ -2570,19 +2690,22 @@
         <v>63</v>
       </c>
       <c r="G46" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H46" t="s">
-        <v>115</v>
+        <v>116</v>
+      </c>
+      <c r="I46" t="s">
+        <v>86</v>
       </c>
       <c r="L46">
         <v>0</v>
       </c>
       <c r="M46" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N46" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="1:15">
@@ -2605,19 +2728,22 @@
         <v>74</v>
       </c>
       <c r="H47" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="I47" t="s">
+        <v>86</v>
       </c>
       <c r="L47">
         <v>0</v>
       </c>
       <c r="M47" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N47" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="O47" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: turn off product
</commit_message>
<xml_diff>
--- a/examples/download.xlsx
+++ b/examples/download.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="199">
   <si>
     <t>訂單號碼
 Số phiếu giao</t>
@@ -1057,7 +1057,7 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1092,7 +1092,7 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1127,7 +1127,7 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1203,7 +1203,7 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1241,7 +1241,7 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1279,7 +1279,7 @@
         <v>21</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1317,7 +1317,7 @@
         <v>22</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1352,7 +1352,7 @@
         <v>23</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1390,7 +1390,7 @@
         <v>24</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1428,7 +1428,7 @@
         <v>25</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1466,7 +1466,7 @@
         <v>26</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1504,7 +1504,7 @@
         <v>27</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1580,7 +1580,7 @@
         <v>29</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1618,7 +1618,7 @@
         <v>30</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1688,7 +1688,7 @@
         <v>32</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1726,7 +1726,7 @@
         <v>33</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1764,7 +1764,7 @@
         <v>34</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1802,7 +1802,7 @@
         <v>35</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1840,7 +1840,7 @@
         <v>36</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1916,7 +1916,7 @@
         <v>38</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1954,7 +1954,7 @@
         <v>39</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1992,7 +1992,7 @@
         <v>40</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2030,7 +2030,7 @@
         <v>41</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2065,7 +2065,7 @@
         <v>42</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2103,7 +2103,7 @@
         <v>43</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2141,7 +2141,7 @@
         <v>44</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2179,7 +2179,7 @@
         <v>45</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2217,7 +2217,7 @@
         <v>46</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2293,7 +2293,7 @@
         <v>48</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2331,7 +2331,7 @@
         <v>49</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2366,7 +2366,7 @@
         <v>50</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2401,7 +2401,7 @@
         <v>51</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2436,7 +2436,7 @@
         <v>52</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2448,6 +2448,9 @@
         <v>61</v>
       </c>
       <c r="G39" t="s">
+        <v>86</v>
+      </c>
+      <c r="H39" t="s">
         <v>86</v>
       </c>
       <c r="I39" t="s">
@@ -2678,7 +2681,7 @@
         <v>59</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46">
         <v>1</v>

</xml_diff>